<commit_message>
Clean up. Removed old comments.
</commit_message>
<xml_diff>
--- a/performance.xlsx
+++ b/performance.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>GPU usage, %</t>
   </si>
@@ -33,7 +33,22 @@
   </si>
   <si>
     <t>2
-Removed recursion return branching</t>
+Removed recursion return branching
+d596716</t>
+  </si>
+  <si>
+    <t>11-17</t>
+  </si>
+  <si>
+    <t>9-17</t>
+  </si>
+  <si>
+    <t>10-19</t>
+  </si>
+  <si>
+    <t>3
+Removed all but 1 IF's
+9e9346d</t>
   </si>
 </sst>
 </file>
@@ -106,7 +121,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -116,13 +131,22 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -428,88 +452,113 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J6"/>
+  <dimension ref="B2:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="7.140625" customWidth="1"/>
+    <col min="6" max="6" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C1" s="1" t="s">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="6" t="s">
+    <row r="4" spans="2:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="2"/>
-      <c r="C4" s="3">
+      <c r="E4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="3">
         <v>512</v>
       </c>
-      <c r="D4" s="2">
+      <c r="C5" s="2">
         <v>40</v>
       </c>
-      <c r="E4" s="2">
+      <c r="D5" s="2">
         <v>9</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C5" s="3">
-        <v>720</v>
-      </c>
-      <c r="D5" s="2">
-        <v>78</v>
-      </c>
       <c r="E5" s="2">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C6" s="3">
-        <v>1024</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" s="2">
-        <v>15</v>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="3">
+        <v>720</v>
+      </c>
+      <c r="C6" s="2">
+        <v>78</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>6</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="3">
+        <v>1024</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2">
+        <v>16</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="8">
+        <v>2048</v>
+      </c>
+      <c r="E8">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="8">
+        <v>4096</v>
+      </c>
+      <c r="E9">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>